<commit_message>
1. 增加alertifyJS 2. 調整網站主題 3. 增加 devHelper(Grid、FormLayout、commonHelper) 4. 增加BA03系列 Controller、view、ViewModel、
</commit_message>
<xml_diff>
--- a/ALMS/SQL/database.xlsx
+++ b/ALMS/SQL/database.xlsx
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>